<commit_message>
update examples for githab
</commit_message>
<xml_diff>
--- a/docs/Входные_данные.xlsx
+++ b/docs/Входные_данные.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ДРОФА\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOIZ\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" tabRatio="893"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35430" windowHeight="16635" tabRatio="893"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="37">
   <si>
     <t>Дата</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>ОСТ.</t>
+  </si>
+  <si>
+    <t>Пласт_1</t>
+  </si>
+  <si>
+    <t>Пласт_1, Пласт_2</t>
+  </si>
+  <si>
+    <t>Месторождение_2</t>
   </si>
 </sst>
 </file>
@@ -536,17 +545,17 @@
   <dimension ref="A1:AA101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="9" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" style="5" bestFit="1" customWidth="1"/>
@@ -658,13 +667,13 @@
         <v>4461</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H2" s="4">
         <v>483718</v>
@@ -732,13 +741,13 @@
         <v>4461</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H3" s="4">
         <v>483718</v>
@@ -806,13 +815,13 @@
         <v>4461</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H4" s="4">
         <v>483718</v>
@@ -880,13 +889,13 @@
         <v>4461</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H5" s="4">
         <v>483718</v>
@@ -954,13 +963,13 @@
         <v>4461</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H6" s="4">
         <v>483718</v>
@@ -1028,13 +1037,13 @@
         <v>4461</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H7" s="4">
         <v>483718</v>
@@ -1102,13 +1111,13 @@
         <v>4461</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H8" s="4">
         <v>483718</v>
@@ -1176,13 +1185,13 @@
         <v>4461</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H9" s="4">
         <v>483718</v>
@@ -1250,13 +1259,13 @@
         <v>4461</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H10" s="4">
         <v>483718</v>
@@ -1324,13 +1333,13 @@
         <v>4461</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H11" s="4">
         <v>483718</v>
@@ -1398,13 +1407,13 @@
         <v>4461</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H12" s="4">
         <v>483718</v>
@@ -1472,13 +1481,13 @@
         <v>4461</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H13" s="4">
         <v>483718</v>
@@ -1546,13 +1555,13 @@
         <v>4461</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H14" s="4">
         <v>483718</v>
@@ -1620,13 +1629,13 @@
         <v>4461</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H15" s="4">
         <v>483718</v>
@@ -1694,13 +1703,13 @@
         <v>4461</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H16" s="4">
         <v>483718</v>
@@ -1768,13 +1777,13 @@
         <v>4461</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H17" s="4">
         <v>483718</v>
@@ -1842,13 +1851,13 @@
         <v>4461</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H18" s="4">
         <v>483718</v>
@@ -1916,13 +1925,13 @@
         <v>4461</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H19" s="4">
         <v>483718</v>
@@ -1990,13 +1999,13 @@
         <v>4461</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H20" s="4">
         <v>483718</v>
@@ -2064,13 +2073,13 @@
         <v>4461</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H21" s="4">
         <v>483718</v>
@@ -2138,13 +2147,13 @@
         <v>4461</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H22" s="4">
         <v>483718</v>
@@ -2212,13 +2221,13 @@
         <v>4461</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H23" s="4">
         <v>483718</v>
@@ -2286,13 +2295,13 @@
         <v>4461</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H24" s="4">
         <v>483718</v>
@@ -2360,13 +2369,13 @@
         <v>4461</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H25" s="4">
         <v>483718</v>
@@ -2434,13 +2443,13 @@
         <v>4461</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H26" s="4">
         <v>483718</v>
@@ -2508,13 +2517,13 @@
         <v>4461</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H27" s="4">
         <v>483718</v>
@@ -2582,13 +2591,13 @@
         <v>4461</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H28" s="4">
         <v>483718</v>
@@ -2656,13 +2665,13 @@
         <v>4461</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H29" s="4">
         <v>483718</v>
@@ -2727,13 +2736,13 @@
         <v>4461</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H30" s="4">
         <v>483718</v>
@@ -2780,13 +2789,13 @@
         <v>4461</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H31" s="4">
         <v>483718</v>
@@ -2845,13 +2854,13 @@
         <v>4461</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H32" s="4">
         <v>483718</v>
@@ -2910,13 +2919,13 @@
         <v>4461</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H33" s="4">
         <v>483718</v>
@@ -2975,13 +2984,13 @@
         <v>4461</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H34" s="4">
         <v>483718</v>
@@ -3040,13 +3049,13 @@
         <v>4461</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H35" s="4">
         <v>483718</v>
@@ -3105,13 +3114,13 @@
         <v>4461</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H36" s="4">
         <v>483718</v>
@@ -3170,13 +3179,13 @@
         <v>4461</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H37" s="4">
         <v>483718</v>
@@ -3235,13 +3244,13 @@
         <v>4461</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H38" s="4">
         <v>483718</v>
@@ -3300,13 +3309,13 @@
         <v>4461</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H39" s="4">
         <v>483718</v>
@@ -3365,13 +3374,13 @@
         <v>4461</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H40" s="4">
         <v>483718</v>
@@ -3430,13 +3439,13 @@
         <v>4461</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H41" s="4">
         <v>483718</v>
@@ -3495,13 +3504,13 @@
         <v>4461</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H42" s="4">
         <v>483718</v>
@@ -3560,13 +3569,13 @@
         <v>4461</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H43" s="4">
         <v>483718</v>
@@ -3625,13 +3634,13 @@
         <v>4461</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H44" s="4">
         <v>483718</v>
@@ -3690,13 +3699,13 @@
         <v>4461</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H45" s="4">
         <v>483718</v>
@@ -3755,13 +3764,13 @@
         <v>4461</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H46" s="4">
         <v>483718</v>
@@ -3820,13 +3829,13 @@
         <v>4461</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E47" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H47" s="4">
         <v>483718</v>
@@ -3885,13 +3894,13 @@
         <v>4461</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H48" s="4">
         <v>483718</v>
@@ -3950,13 +3959,13 @@
         <v>4461</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H49" s="4">
         <v>483718</v>
@@ -4015,13 +4024,13 @@
         <v>4461</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H50" s="4">
         <v>483718</v>
@@ -4080,13 +4089,13 @@
         <v>4461</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H51" s="4">
         <v>483718</v>
@@ -4145,13 +4154,13 @@
         <v>4461</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E52" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H52" s="4">
         <v>483718</v>
@@ -4210,13 +4219,13 @@
         <v>4461</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E53" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H53" s="4">
         <v>483718</v>
@@ -4275,13 +4284,13 @@
         <v>4461</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E54" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H54" s="4">
         <v>483718</v>
@@ -4340,13 +4349,13 @@
         <v>4461</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H55" s="4">
         <v>483718</v>
@@ -4405,13 +4414,13 @@
         <v>4461</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E56" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H56" s="4">
         <v>483718</v>
@@ -4470,13 +4479,13 @@
         <v>4461</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H57" s="4">
         <v>483718</v>
@@ -4535,13 +4544,13 @@
         <v>4461</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H58" s="4">
         <v>483718</v>
@@ -4600,13 +4609,13 @@
         <v>4461</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E59" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H59" s="4">
         <v>483718</v>
@@ -4665,13 +4674,13 @@
         <v>4461</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E60" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H60" s="4">
         <v>483718</v>
@@ -4730,13 +4739,13 @@
         <v>4461</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E61" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H61" s="4">
         <v>483718</v>
@@ -4795,13 +4804,13 @@
         <v>4461</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E62" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H62" s="4">
         <v>483718</v>
@@ -4860,13 +4869,13 @@
         <v>4461</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E63" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H63" s="4">
         <v>483718</v>
@@ -4925,13 +4934,13 @@
         <v>4461</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E64" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H64" s="4">
         <v>483718</v>
@@ -4990,13 +4999,13 @@
         <v>4461</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H65" s="4">
         <v>483718</v>
@@ -5055,13 +5064,13 @@
         <v>4461</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E66" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H66" s="4">
         <v>483718</v>
@@ -5120,13 +5129,13 @@
         <v>4461</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H67" s="4">
         <v>483718</v>
@@ -5185,13 +5194,13 @@
         <v>4461</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E68" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H68" s="4">
         <v>483718</v>
@@ -5250,13 +5259,13 @@
         <v>4461</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E69" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H69" s="4">
         <v>483718</v>
@@ -5315,13 +5324,13 @@
         <v>4461</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E70" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H70" s="4">
         <v>483718</v>
@@ -5380,13 +5389,13 @@
         <v>4461</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E71" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H71" s="4">
         <v>483718</v>
@@ -5445,13 +5454,13 @@
         <v>4461</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E72" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H72" s="4">
         <v>483718</v>
@@ -5510,13 +5519,13 @@
         <v>4461</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E73" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H73" s="4">
         <v>483718</v>
@@ -5575,13 +5584,13 @@
         <v>4461</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E74" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H74" s="4">
         <v>483718</v>
@@ -5640,13 +5649,13 @@
         <v>4461</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E75" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H75" s="4">
         <v>483718</v>
@@ -5705,13 +5714,13 @@
         <v>4461</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E76" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H76" s="4">
         <v>483718</v>
@@ -5770,13 +5779,13 @@
         <v>4461</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E77" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H77" s="4">
         <v>483718</v>
@@ -5835,13 +5844,13 @@
         <v>4461</v>
       </c>
       <c r="C78" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E78" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H78" s="4">
         <v>483718</v>
@@ -5900,13 +5909,13 @@
         <v>4461</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E79" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H79" s="4">
         <v>483718</v>
@@ -5965,13 +5974,13 @@
         <v>4461</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E80" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H80" s="4">
         <v>483718</v>
@@ -6030,13 +6039,13 @@
         <v>4461</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E81" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H81" s="4">
         <v>483718</v>
@@ -6095,13 +6104,13 @@
         <v>4461</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E82" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H82" s="4">
         <v>483718</v>
@@ -6160,13 +6169,13 @@
         <v>4461</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E83" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H83" s="4">
         <v>483718</v>
@@ -6225,13 +6234,13 @@
         <v>4461</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E84" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H84" s="4">
         <v>483718</v>
@@ -6290,13 +6299,13 @@
         <v>4461</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E85" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H85" s="4">
         <v>483718</v>
@@ -6355,13 +6364,13 @@
         <v>4461</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E86" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H86" s="4">
         <v>483718</v>
@@ -6420,13 +6429,13 @@
         <v>4461</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E87" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H87" s="4">
         <v>483718</v>
@@ -6485,13 +6494,13 @@
         <v>4461</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E88" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H88" s="4">
         <v>483718</v>
@@ -6550,13 +6559,13 @@
         <v>4461</v>
       </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E89" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H89" s="4">
         <v>483718</v>
@@ -6615,13 +6624,13 @@
         <v>4461</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E90" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H90" s="4">
         <v>483718</v>
@@ -6680,13 +6689,13 @@
         <v>4461</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E91" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H91" s="4">
         <v>483718</v>
@@ -6745,13 +6754,13 @@
         <v>4461</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E92" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H92" s="4">
         <v>483718</v>
@@ -6810,13 +6819,13 @@
         <v>4461</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E93" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H93" s="4">
         <v>483718</v>
@@ -6875,13 +6884,13 @@
         <v>4461</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E94" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H94" s="4">
         <v>483718</v>
@@ -6940,13 +6949,13 @@
         <v>4461</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E95" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H95" s="4">
         <v>483718</v>
@@ -7005,13 +7014,13 @@
         <v>4461</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E96" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H96" s="4">
         <v>483718</v>
@@ -7070,13 +7079,13 @@
         <v>4461</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E97" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H97" s="4">
         <v>483718</v>
@@ -7135,13 +7144,13 @@
         <v>4461</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E98" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H98" s="4">
         <v>483718</v>
@@ -7200,13 +7209,13 @@
         <v>4461</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E99" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H99" s="4">
         <v>483718</v>
@@ -7265,13 +7274,13 @@
         <v>4461</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E100" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H100" s="4">
         <v>483718</v>
@@ -7330,13 +7339,13 @@
         <v>4461</v>
       </c>
       <c r="C101" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E101" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H101" s="4">
         <v>483718</v>

</xml_diff>